<commit_message>
added singed pdf and latex code
</commit_message>
<xml_diff>
--- a/ResearchDiary/Questionnaires/NASA-TLX-Calculator.xlsx
+++ b/ResearchDiary/Questionnaires/NASA-TLX-Calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmaer\Documents\FH\Projects\MasterArbeit\mmt-masterarbeit-david-maerzendorfer\ResearchDiary\Questionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5290BFEB-848B-4924-A0A4-FBB61FBFA169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA306669-72F8-4BEF-A3BC-8671778F2FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
   <si>
     <t>Mental Demand</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>hover</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -958,27 +961,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -988,6 +970,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,6 +980,90 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1023,72 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2673,40 +2676,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="31.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="107"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="100"/>
     </row>
     <row r="2" spans="1:38" ht="26.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
     </row>
     <row r="3" spans="1:38" ht="7.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="47"/>
@@ -2771,66 +2774,66 @@
     </row>
     <row r="6" spans="1:38" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="103">
+      <c r="B6" s="101">
         <v>1</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="109">
+      <c r="C6" s="105"/>
+      <c r="D6" s="103">
         <v>2</v>
       </c>
-      <c r="E6" s="110"/>
-      <c r="F6" s="103">
+      <c r="E6" s="104"/>
+      <c r="F6" s="101">
         <v>3</v>
       </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109">
+      <c r="G6" s="102"/>
+      <c r="H6" s="103">
         <v>4</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="100">
+      <c r="I6" s="104"/>
+      <c r="J6" s="106">
         <v>5</v>
       </c>
-      <c r="K6" s="101"/>
-      <c r="L6" s="98">
+      <c r="K6" s="107"/>
+      <c r="L6" s="108">
         <v>6</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100">
+      <c r="M6" s="109"/>
+      <c r="N6" s="106">
         <v>7</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="98">
+      <c r="O6" s="107"/>
+      <c r="P6" s="108">
         <v>8</v>
       </c>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="103">
+      <c r="Q6" s="109"/>
+      <c r="R6" s="101">
         <v>9</v>
       </c>
-      <c r="S6" s="108"/>
-      <c r="T6" s="109">
+      <c r="S6" s="102"/>
+      <c r="T6" s="103">
         <v>10</v>
       </c>
-      <c r="U6" s="110"/>
-      <c r="V6" s="103">
+      <c r="U6" s="104"/>
+      <c r="V6" s="101">
         <v>11</v>
       </c>
-      <c r="W6" s="108"/>
-      <c r="X6" s="109">
+      <c r="W6" s="102"/>
+      <c r="X6" s="103">
         <v>12</v>
       </c>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="103">
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="101">
         <v>13</v>
       </c>
-      <c r="AA6" s="108"/>
-      <c r="AB6" s="109">
+      <c r="AA6" s="102"/>
+      <c r="AB6" s="103">
         <v>14</v>
       </c>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="103">
+      <c r="AC6" s="104"/>
+      <c r="AD6" s="101">
         <v>15</v>
       </c>
-      <c r="AE6" s="104"/>
+      <c r="AE6" s="105"/>
       <c r="AG6" s="34" t="s">
         <v>10</v>
       </c>
@@ -9547,6 +9550,9 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="AB6:AC6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="R6:S6"/>
     <mergeCell ref="T6:U6"/>
@@ -9561,9 +9567,6 @@
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="A2:N2"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="AB6:AC6"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:AE118">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
@@ -9585,14 +9588,14 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:X173"/>
+  <dimension ref="A1:Y173"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <pane xSplit="19" ySplit="12" topLeftCell="T13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I13" sqref="I13"/>
       <selection pane="topRight" activeCell="I13" sqref="I13"/>
       <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
-      <selection pane="bottomRight" activeCell="Z20" sqref="Z20"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9634,77 +9637,77 @@
     <col min="41" max="41" width="4.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:25" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
-      <c r="T1" s="122" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="100"/>
+      <c r="T1" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="124"/>
-    </row>
-    <row r="2" spans="1:24" ht="24.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="120"/>
+    </row>
+    <row r="2" spans="1:25" ht="24.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="48" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="45"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="127"/>
-    </row>
-    <row r="3" spans="1:24" s="64" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T2" s="121"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="123"/>
+    </row>
+    <row r="3" spans="1:25" s="64" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="45"/>
       <c r="O3" s="65"/>
       <c r="P3" s="65"/>
-      <c r="T3" s="118" t="s">
+      <c r="T3" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="119"/>
+      <c r="U3" s="141"/>
       <c r="V3" s="70"/>
-      <c r="W3" s="116" t="s">
+      <c r="W3" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="117"/>
-    </row>
-    <row r="4" spans="1:24" s="64" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="139" t="s">
+      <c r="X3" s="139"/>
+    </row>
+    <row r="4" spans="1:25" s="64" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="140"/>
-      <c r="I4" s="140"/>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="141"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
       <c r="T4" s="73" t="s">
         <v>16</v>
       </c>
@@ -9720,8 +9723,12 @@
         <f>AVERAGE(B13:G25)</f>
         <v>37.916666666666664</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" s="62" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y4" s="64">
+        <f>STDEV(X7:X12)</f>
+        <v>10.696406776186144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="62" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="67"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
@@ -9746,7 +9753,7 @@
       <c r="W5" s="77"/>
       <c r="X5" s="78"/>
     </row>
-    <row r="6" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="42"/>
       <c r="B6" s="60" t="s">
         <v>23</v>
@@ -9766,29 +9773,32 @@
       <c r="G6" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="138"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="138"/>
-      <c r="T6" s="111" t="s">
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="T6" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="U6" s="112"/>
+      <c r="U6" s="134"/>
       <c r="V6" s="72"/>
-      <c r="W6" s="114" t="s">
+      <c r="W6" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="X6" s="115"/>
-    </row>
-    <row r="7" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="X6" s="137"/>
+      <c r="Y6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="41"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42"/>
@@ -9796,20 +9806,20 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="127"/>
+      <c r="N7" s="127"/>
+      <c r="O7" s="127"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="132" t="s">
+      <c r="Q7" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="132"/>
+      <c r="R7" s="126"/>
       <c r="T7" s="79" t="s">
         <v>7</v>
       </c>
@@ -9825,43 +9835,47 @@
         <f>AVERAGEIF($B$13:$B$123,"&gt;0")</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y7">
+        <f>STDEV(B13:B24)</f>
+        <v>21.105794120443452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="41"/>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="120" t="s">
+      <c r="E8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="120" t="s">
+      <c r="F8" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="120" t="s">
+      <c r="G8" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="130" t="s">
+      <c r="I8" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="130" t="s">
+      <c r="J8" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="130" t="s">
+      <c r="K8" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="130" t="s">
+      <c r="L8" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="130" t="s">
+      <c r="M8" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="130" t="s">
+      <c r="N8" s="116" t="s">
         <v>5</v>
       </c>
       <c r="O8" s="38"/>
@@ -9883,29 +9897,33 @@
         <f>AVERAGEIF($C$13:$C$123,"&gt;0")</f>
         <v>20.454545454545453</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="120" t="s">
+      <c r="Y8">
+        <f>STDEV(C13:C24)</f>
+        <v>17.336902313221408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="136" t="s">
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="130" t="s">
         <v>35</v>
       </c>
       <c r="P9" s="37"/>
       <c r="Q9" s="66"/>
-      <c r="R9" s="128" t="s">
+      <c r="R9" s="124" t="s">
         <v>35</v>
       </c>
       <c r="T9" s="79" t="s">
@@ -9923,25 +9941,29 @@
         <f>AVERAGEIF($D$13:$E$123,"&gt;0")</f>
         <v>36.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="120"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="136"/>
+      <c r="Y9">
+        <f>STDEV(D13:D24)</f>
+        <v>24.629835319765903</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="114"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
+      <c r="K10" s="116"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="130"/>
       <c r="P10" s="37"/>
       <c r="Q10" s="66"/>
-      <c r="R10" s="128"/>
+      <c r="R10" s="124"/>
       <c r="T10" s="79" t="s">
         <v>4</v>
       </c>
@@ -9957,25 +9979,29 @@
         <f>AVERAGEIF($E$13:$E$123,"&gt;0")</f>
         <v>42.916666666666664</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="120"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="I11" s="130"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="130"/>
-      <c r="M11" s="130"/>
-      <c r="N11" s="130"/>
-      <c r="O11" s="136"/>
+      <c r="Y10">
+        <f>STDEV(E13:E24)</f>
+        <v>22.305557127941881</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="114"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="116"/>
+      <c r="M11" s="116"/>
+      <c r="N11" s="116"/>
+      <c r="O11" s="130"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="134"/>
-      <c r="R11" s="128"/>
+      <c r="Q11" s="128"/>
+      <c r="R11" s="124"/>
       <c r="T11" s="79" t="s">
         <v>3</v>
       </c>
@@ -9991,25 +10017,29 @@
         <f>AVERAGEIF($F$13:$F$122,"&gt;0")</f>
         <v>43.75</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="121"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="137"/>
+      <c r="Y11">
+        <f>STDEV(F13:F24)</f>
+        <v>23.269664216040436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="115"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="117"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="131"/>
       <c r="P12" s="40"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="129"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="125"/>
       <c r="T12" s="81" t="s">
         <v>5</v>
       </c>
@@ -10025,8 +10055,12 @@
         <f>AVERAGEIF($G$13:$G$122,"&gt;0")</f>
         <v>52.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y12">
+        <f>STDEV(G13:G24)</f>
+        <v>30.413812651491099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="50" t="s">
         <v>45</v>
       </c>
@@ -10083,10 +10117,10 @@
         <f t="shared" ref="R13:R25" si="0">AVERAGE(B13:G13)</f>
         <v>45</v>
       </c>
-      <c r="W13" s="113"/>
-      <c r="X13" s="113"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W13" s="135"/>
+      <c r="X13" s="135"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
         <v>46</v>
       </c>
@@ -10145,7 +10179,7 @@
       <c r="W14" s="58"/>
       <c r="X14" s="58"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>47</v>
       </c>
@@ -10204,7 +10238,7 @@
       <c r="W15" s="58"/>
       <c r="X15" s="58"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>48</v>
       </c>
@@ -15298,12 +15332,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="G8:G12"/>
-    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="T3:U3"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="T1:X2"/>
     <mergeCell ref="R9:R12"/>
@@ -15320,11 +15353,12 @@
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="I8:I12"/>
     <mergeCell ref="J8:J12"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="K8:K12"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:G123">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
@@ -15394,40 +15428,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="31.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="107"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="100"/>
     </row>
     <row r="2" spans="1:38" ht="26.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="110"/>
+      <c r="M2" s="110"/>
+      <c r="N2" s="110"/>
     </row>
     <row r="3" spans="1:38" ht="7.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="47"/>
@@ -15492,66 +15526,66 @@
     </row>
     <row r="6" spans="1:38" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
-      <c r="B6" s="103">
+      <c r="B6" s="101">
         <v>1</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="109">
+      <c r="C6" s="105"/>
+      <c r="D6" s="103">
         <v>2</v>
       </c>
-      <c r="E6" s="110"/>
-      <c r="F6" s="103">
+      <c r="E6" s="104"/>
+      <c r="F6" s="101">
         <v>3</v>
       </c>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109">
+      <c r="G6" s="102"/>
+      <c r="H6" s="103">
         <v>4</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="100">
+      <c r="I6" s="104"/>
+      <c r="J6" s="106">
         <v>5</v>
       </c>
-      <c r="K6" s="101"/>
-      <c r="L6" s="98">
+      <c r="K6" s="107"/>
+      <c r="L6" s="108">
         <v>6</v>
       </c>
-      <c r="M6" s="99"/>
-      <c r="N6" s="100">
+      <c r="M6" s="109"/>
+      <c r="N6" s="106">
         <v>7</v>
       </c>
-      <c r="O6" s="101"/>
-      <c r="P6" s="98">
+      <c r="O6" s="107"/>
+      <c r="P6" s="108">
         <v>8</v>
       </c>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="103">
+      <c r="Q6" s="109"/>
+      <c r="R6" s="101">
         <v>9</v>
       </c>
-      <c r="S6" s="108"/>
-      <c r="T6" s="109">
+      <c r="S6" s="102"/>
+      <c r="T6" s="103">
         <v>10</v>
       </c>
-      <c r="U6" s="110"/>
-      <c r="V6" s="103">
+      <c r="U6" s="104"/>
+      <c r="V6" s="101">
         <v>11</v>
       </c>
-      <c r="W6" s="108"/>
-      <c r="X6" s="109">
+      <c r="W6" s="102"/>
+      <c r="X6" s="103">
         <v>12</v>
       </c>
-      <c r="Y6" s="110"/>
-      <c r="Z6" s="103">
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="101">
         <v>13</v>
       </c>
-      <c r="AA6" s="108"/>
-      <c r="AB6" s="109">
+      <c r="AA6" s="102"/>
+      <c r="AB6" s="103">
         <v>14</v>
       </c>
-      <c r="AC6" s="110"/>
-      <c r="AD6" s="103">
+      <c r="AC6" s="104"/>
+      <c r="AD6" s="101">
         <v>15</v>
       </c>
-      <c r="AE6" s="104"/>
+      <c r="AE6" s="105"/>
       <c r="AG6" s="34" t="s">
         <v>10</v>
       </c>
@@ -22268,6 +22302,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="B6:C6"/>
@@ -22277,14 +22319,6 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N6:O6"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:AE118">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
@@ -22306,14 +22340,14 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:X173"/>
+  <dimension ref="A1:Y173"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <pane xSplit="19" ySplit="12" topLeftCell="T13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="I13" sqref="I13"/>
       <selection pane="topRight" activeCell="I13" sqref="I13"/>
       <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
-      <selection pane="bottomRight" activeCell="Y25" sqref="Y25"/>
+      <selection pane="bottomRight" activeCell="Y4" sqref="Y4:Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22355,77 +22389,77 @@
     <col min="41" max="41" width="4.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:25" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="107"/>
-      <c r="T1" s="122" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="100"/>
+      <c r="T1" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="124"/>
-    </row>
-    <row r="2" spans="1:24" ht="24.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="120"/>
+    </row>
+    <row r="2" spans="1:25" ht="24.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="48" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="45"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="127"/>
-    </row>
-    <row r="3" spans="1:24" s="64" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="T2" s="121"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="122"/>
+      <c r="W2" s="122"/>
+      <c r="X2" s="123"/>
+    </row>
+    <row r="3" spans="1:25" s="64" customFormat="1" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="45"/>
       <c r="O3" s="65"/>
       <c r="P3" s="65"/>
-      <c r="T3" s="118" t="s">
+      <c r="T3" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="119"/>
+      <c r="U3" s="141"/>
       <c r="V3" s="70"/>
-      <c r="W3" s="116" t="s">
+      <c r="W3" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="117"/>
-    </row>
-    <row r="4" spans="1:24" s="64" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="139" t="s">
+      <c r="X3" s="139"/>
+    </row>
+    <row r="4" spans="1:25" s="64" customFormat="1" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="140"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="140"/>
-      <c r="I4" s="140"/>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
-      <c r="O4" s="140"/>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="141"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
       <c r="T4" s="73" t="s">
         <v>16</v>
       </c>
@@ -22441,8 +22475,12 @@
         <f>AVERAGE(B13:G25)</f>
         <v>27.013888888888889</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" s="62" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y4" s="64">
+        <f>STDEV(X7:X12)</f>
+        <v>6.5046456285947434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="62" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="67"/>
       <c r="B5" s="67"/>
       <c r="C5" s="67"/>
@@ -22467,7 +22505,7 @@
       <c r="W5" s="77"/>
       <c r="X5" s="78"/>
     </row>
-    <row r="6" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="42"/>
       <c r="B6" s="60" t="s">
         <v>23</v>
@@ -22487,29 +22525,32 @@
       <c r="G6" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="138" t="s">
+      <c r="I6" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="138"/>
-      <c r="K6" s="138"/>
-      <c r="L6" s="138"/>
-      <c r="M6" s="138"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="138"/>
-      <c r="P6" s="138"/>
-      <c r="Q6" s="138"/>
-      <c r="R6" s="138"/>
-      <c r="T6" s="111" t="s">
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="T6" s="133" t="s">
         <v>40</v>
       </c>
-      <c r="U6" s="112"/>
+      <c r="U6" s="134"/>
       <c r="V6" s="72"/>
-      <c r="W6" s="114" t="s">
+      <c r="W6" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="X6" s="115"/>
-    </row>
-    <row r="7" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="X6" s="137"/>
+      <c r="Y6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="41"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42"/>
@@ -22517,20 +22558,20 @@
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
-      <c r="M7" s="133"/>
-      <c r="N7" s="133"/>
-      <c r="O7" s="133"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="127"/>
+      <c r="N7" s="127"/>
+      <c r="O7" s="127"/>
       <c r="P7" s="37"/>
-      <c r="Q7" s="132" t="s">
+      <c r="Q7" s="126" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="132"/>
+      <c r="R7" s="126"/>
       <c r="T7" s="79" t="s">
         <v>7</v>
       </c>
@@ -22546,43 +22587,47 @@
         <f>AVERAGEIF($B$13:$B$123,"&gt;0")</f>
         <v>36.666666666666664</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y7">
+        <f>STDEV(B13:B24)</f>
+        <v>24.24621182533032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="41"/>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="120" t="s">
+      <c r="C8" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="120" t="s">
+      <c r="E8" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="120" t="s">
+      <c r="F8" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="120" t="s">
+      <c r="G8" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="130" t="s">
+      <c r="I8" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="130" t="s">
+      <c r="J8" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="130" t="s">
+      <c r="K8" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="130" t="s">
+      <c r="L8" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="130" t="s">
+      <c r="M8" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="130" t="s">
+      <c r="N8" s="116" t="s">
         <v>5</v>
       </c>
       <c r="O8" s="38"/>
@@ -22604,29 +22649,33 @@
         <f>AVERAGEIF($C$13:$C$123,"&gt;0")</f>
         <v>16.818181818181817</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="120" t="s">
+      <c r="Y8">
+        <f>STDEV(C13:C24)</f>
+        <v>17.117021476951656</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="136" t="s">
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="I9" s="116"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
+      <c r="M9" s="116"/>
+      <c r="N9" s="116"/>
+      <c r="O9" s="130" t="s">
         <v>35</v>
       </c>
       <c r="P9" s="37"/>
       <c r="Q9" s="66"/>
-      <c r="R9" s="128" t="s">
+      <c r="R9" s="124" t="s">
         <v>35</v>
       </c>
       <c r="T9" s="79" t="s">
@@ -22644,25 +22693,29 @@
         <f>AVERAGEIF($D$13:$E$123,"&gt;0")</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="120"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="130"/>
-      <c r="K10" s="130"/>
-      <c r="L10" s="130"/>
-      <c r="M10" s="130"/>
-      <c r="N10" s="130"/>
-      <c r="O10" s="136"/>
+      <c r="Y9">
+        <f>STDEV(D13:D24)</f>
+        <v>27.561913774429577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="114"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
+      <c r="K10" s="116"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="130"/>
       <c r="P10" s="37"/>
       <c r="Q10" s="66"/>
-      <c r="R10" s="128"/>
+      <c r="R10" s="124"/>
       <c r="T10" s="79" t="s">
         <v>4</v>
       </c>
@@ -22678,25 +22731,29 @@
         <f>AVERAGEIF($E$13:$E$123,"&gt;0")</f>
         <v>25.90909090909091</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="120"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="I11" s="130"/>
-      <c r="J11" s="130"/>
-      <c r="K11" s="130"/>
-      <c r="L11" s="130"/>
-      <c r="M11" s="130"/>
-      <c r="N11" s="130"/>
-      <c r="O11" s="136"/>
+      <c r="Y10">
+        <f>STDEV(E13:E24)</f>
+        <v>18.964680089816724</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="114"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="114"/>
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="114"/>
+      <c r="I11" s="116"/>
+      <c r="J11" s="116"/>
+      <c r="K11" s="116"/>
+      <c r="L11" s="116"/>
+      <c r="M11" s="116"/>
+      <c r="N11" s="116"/>
+      <c r="O11" s="130"/>
       <c r="P11" s="37"/>
-      <c r="Q11" s="134"/>
-      <c r="R11" s="128"/>
+      <c r="Q11" s="128"/>
+      <c r="R11" s="124"/>
       <c r="T11" s="79" t="s">
         <v>3</v>
       </c>
@@ -22712,25 +22769,29 @@
         <f>AVERAGEIF($F$13:$F$123,"&gt;0")</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="121"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="121"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="I12" s="131"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="131"/>
-      <c r="L12" s="131"/>
-      <c r="M12" s="131"/>
-      <c r="N12" s="131"/>
-      <c r="O12" s="137"/>
+      <c r="Y11">
+        <f>STDEV(F13:F24)</f>
+        <v>16.376257758774383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="115"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="117"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="131"/>
       <c r="P12" s="40"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="129"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="125"/>
       <c r="T12" s="81" t="s">
         <v>5</v>
       </c>
@@ -22746,8 +22807,12 @@
         <f>AVERAGEIF($G$13:$G$123,"&gt;0")</f>
         <v>27.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y12">
+        <f>STDEV(G13:G24)</f>
+        <v>24.541245430351069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="50" t="s">
         <v>45</v>
       </c>
@@ -22804,10 +22869,10 @@
         <f>AVERAGE(B13:G13)</f>
         <v>46.666666666666664</v>
       </c>
-      <c r="W13" s="113"/>
-      <c r="X13" s="113"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W13" s="135"/>
+      <c r="X13" s="135"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
         <v>46</v>
       </c>
@@ -22866,7 +22931,7 @@
       <c r="W14" s="58"/>
       <c r="X14" s="58"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>47</v>
       </c>
@@ -22925,7 +22990,7 @@
       <c r="W15" s="58"/>
       <c r="X15" s="58"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>48</v>
       </c>
@@ -28019,14 +28084,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="I6:R6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="T1:X2"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="L8:L12"/>
+    <mergeCell ref="M8:M12"/>
+    <mergeCell ref="N8:N12"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="O9:O12"/>
     <mergeCell ref="I7:O7"/>
@@ -28041,11 +28103,14 @@
     <mergeCell ref="J8:J12"/>
     <mergeCell ref="R9:R12"/>
     <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="K8:K12"/>
-    <mergeCell ref="L8:L12"/>
-    <mergeCell ref="M8:M12"/>
-    <mergeCell ref="N8:N12"/>
+    <mergeCell ref="I6:R6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="T1:X2"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="B4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="B15:G123">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
@@ -28069,7 +28134,7 @@
   </sheetPr>
   <dimension ref="E14:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>

</xml_diff>